<commit_message>
can now add behavior from flashingstim_2P_Frames to summary figs - AW
</commit_message>
<xml_diff>
--- a/BehaviorAnalysis/AW analysis/catch trials figs/catch-days.xlsx
+++ b/BehaviorAnalysis/AW analysis/catch trials figs/catch-days.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="14">
   <si>
     <t>Subject</t>
   </si>
@@ -61,7 +61,13 @@
     <t>100:end</t>
   </si>
   <si>
+    <t>1:200</t>
+  </si>
+  <si>
     <t>1:250</t>
+  </si>
+  <si>
+    <t>1:150</t>
   </si>
 </sst>
 </file>
@@ -403,19 +409,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -434,97 +437,97 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B2">
-        <v>150726</v>
+        <v>150723</v>
       </c>
       <c r="C2">
-        <v>1240</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+        <v>1039</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B3">
-        <v>150728</v>
+        <v>150727</v>
       </c>
       <c r="C3">
-        <v>932</v>
+        <v>852</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B4">
-        <v>150729</v>
+        <v>150728</v>
       </c>
       <c r="C4">
-        <v>907</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
+        <v>934</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B5">
         <v>150730</v>
       </c>
       <c r="C5">
-        <v>1038</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
+        <v>1040</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B6">
         <v>150731</v>
       </c>
       <c r="C6">
-        <v>849</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
+        <v>852</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>614</v>
-      </c>
-      <c r="B7" s="7">
+        <v>613</v>
+      </c>
+      <c r="B7" s="4">
         <v>150803</v>
       </c>
       <c r="C7" s="5">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>614</v>
-      </c>
-      <c r="B8" s="7">
+        <v>613</v>
+      </c>
+      <c r="B8" s="4">
         <v>150804</v>
       </c>
       <c r="C8" s="5">
-        <v>907</v>
+        <v>1036</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
@@ -532,97 +535,97 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B9" s="4">
-        <v>150806</v>
+        <v>150805</v>
       </c>
       <c r="C9" s="5">
-        <v>1027</v>
+        <v>926</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B10" s="4">
-        <v>150807</v>
+        <v>150806</v>
       </c>
       <c r="C10" s="5">
-        <v>906</v>
+        <v>1030</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B11" s="4">
-        <v>150824</v>
+        <v>150807</v>
       </c>
       <c r="C11" s="5">
-        <v>1215</v>
+        <v>909</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>614</v>
-      </c>
-      <c r="B12" s="2">
-        <v>150827</v>
+        <v>613</v>
+      </c>
+      <c r="B12" s="7">
+        <v>150825</v>
       </c>
       <c r="C12" s="5">
-        <v>1035</v>
+        <v>1013</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>614</v>
-      </c>
-      <c r="B13" s="2">
-        <v>150829</v>
+        <v>613</v>
+      </c>
+      <c r="B13" s="4">
+        <v>150828</v>
       </c>
       <c r="C13" s="5">
-        <v>1420</v>
+        <v>1233</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>614</v>
-      </c>
-      <c r="B14" s="2">
-        <v>150901</v>
+        <v>613</v>
+      </c>
+      <c r="B14" s="4">
+        <v>150831</v>
       </c>
       <c r="C14" s="5">
-        <v>1008</v>
+        <v>1210</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>614</v>
-      </c>
-      <c r="B15" s="2">
-        <v>150903</v>
+        <v>613</v>
+      </c>
+      <c r="B15" s="4">
+        <v>150902</v>
       </c>
       <c r="C15" s="5">
-        <v>1019</v>
+        <v>1206</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
@@ -630,235 +633,267 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>614</v>
-      </c>
-      <c r="B16" s="2">
-        <v>150905</v>
+        <v>613</v>
+      </c>
+      <c r="B16" s="4">
+        <v>150904</v>
       </c>
       <c r="C16" s="5">
-        <v>1416</v>
+        <v>1211</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>614</v>
-      </c>
-      <c r="B17" s="2">
-        <v>150908</v>
+        <v>613</v>
+      </c>
+      <c r="B17" s="4">
+        <v>150907</v>
       </c>
       <c r="C17" s="5">
-        <v>1002</v>
+        <v>1214</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="3">
+        <v>613</v>
+      </c>
+      <c r="B18" s="7">
+        <v>150810</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1441</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="3">
+        <v>613</v>
+      </c>
+      <c r="B19" s="7">
+        <v>150810</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1516</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="3">
+        <v>613</v>
+      </c>
+      <c r="B20" s="7">
+        <v>150811</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1233</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="3">
+        <v>613</v>
+      </c>
+      <c r="B21" s="7">
+        <v>150811</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1307</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="3">
+        <v>613</v>
+      </c>
+      <c r="B22" s="7">
+        <v>150812</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1307</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="3">
+        <v>613</v>
+      </c>
+      <c r="B23" s="7">
+        <v>150812</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1343</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="3">
+        <v>613</v>
+      </c>
+      <c r="B24" s="7">
+        <v>150813</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1646</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="3">
+        <v>613</v>
+      </c>
+      <c r="B25" s="7">
+        <v>150817</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1253</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="3">
+        <v>613</v>
+      </c>
+      <c r="B26" s="7">
+        <v>150817</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1333</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="3">
+        <v>613</v>
+      </c>
+      <c r="B27" s="7">
+        <v>150818</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1259</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="5"/>
+      <c r="A28" s="3">
+        <v>613</v>
+      </c>
+      <c r="B28" s="7">
+        <v>150818</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1335</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="3">
+        <v>613</v>
+      </c>
+      <c r="B29" s="7">
+        <v>150819</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1151</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="3">
+        <v>613</v>
+      </c>
+      <c r="B30" s="7">
+        <v>150820</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1612</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="3">
+        <v>613</v>
+      </c>
+      <c r="B31" s="7">
+        <v>150820</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1653</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="C68" s="5"/>
+      <c r="A32" s="3">
+        <v>613</v>
+      </c>
+      <c r="B32" s="7">
+        <v>150821</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1224</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>613</v>
+      </c>
+      <c r="B33" s="7">
+        <v>150821</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1301</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:D12">
@@ -874,11 +909,13 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -945,7 +982,7 @@
       <c r="C2">
         <v>1240</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3">
@@ -993,7 +1030,7 @@
         <v>852</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
@@ -1015,7 +1052,7 @@
       <c r="C4">
         <v>907</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3">
@@ -1050,7 +1087,7 @@
       <c r="C5">
         <v>1038</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="3">
@@ -1085,7 +1122,7 @@
       <c r="C6">
         <v>849</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="3">
@@ -1098,7 +1135,7 @@
         <v>852</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
@@ -1254,14 +1291,14 @@
       <c r="A11" s="3">
         <v>614</v>
       </c>
-      <c r="B11" s="4">
-        <v>150824</v>
+      <c r="B11" s="2">
+        <v>150810</v>
       </c>
       <c r="C11" s="5">
-        <v>1215</v>
+        <v>1333</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F11" s="3">
         <v>613</v>
@@ -1290,13 +1327,13 @@
         <v>614</v>
       </c>
       <c r="B12" s="2">
-        <v>150827</v>
+        <v>150811</v>
       </c>
       <c r="C12" s="5">
-        <v>1035</v>
+        <v>1115</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
         <v>613</v>
@@ -1325,13 +1362,13 @@
         <v>614</v>
       </c>
       <c r="B13" s="2">
-        <v>150829</v>
+        <v>150811</v>
       </c>
       <c r="C13" s="5">
-        <v>1420</v>
+        <v>1151</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3">
         <v>613</v>
@@ -1360,13 +1397,13 @@
         <v>614</v>
       </c>
       <c r="B14" s="2">
-        <v>150901</v>
+        <v>150812</v>
       </c>
       <c r="C14" s="5">
-        <v>1008</v>
+        <v>1137</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F14" s="3">
         <v>613</v>
@@ -1395,10 +1432,10 @@
         <v>614</v>
       </c>
       <c r="B15" s="2">
-        <v>150903</v>
+        <v>150812</v>
       </c>
       <c r="C15" s="5">
-        <v>1019</v>
+        <v>1217</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
@@ -1430,10 +1467,10 @@
         <v>614</v>
       </c>
       <c r="B16" s="2">
-        <v>150905</v>
+        <v>150813</v>
       </c>
       <c r="C16" s="5">
-        <v>1416</v>
+        <v>1450</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>4</v>
@@ -1465,13 +1502,13 @@
         <v>614</v>
       </c>
       <c r="B17" s="2">
-        <v>150908</v>
+        <v>150813</v>
       </c>
       <c r="C17" s="5">
-        <v>1002</v>
+        <v>1527</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F17" s="3">
         <v>613</v>
@@ -1496,7 +1533,30 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
+      <c r="A18" s="3">
+        <v>614</v>
+      </c>
+      <c r="B18" s="2">
+        <v>150814</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1103</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3">
+        <v>613</v>
+      </c>
+      <c r="G18" s="7">
+        <v>150810</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1441</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1508,7 +1568,30 @@
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
+      <c r="A19" s="3">
+        <v>614</v>
+      </c>
+      <c r="B19" s="2">
+        <v>150814</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1139</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>613</v>
+      </c>
+      <c r="G19" s="7">
+        <v>150810</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1516</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K19" s="3"/>
       <c r="L19" s="2"/>
       <c r="M19" s="5"/>
@@ -1520,7 +1603,30 @@
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
+      <c r="A20" s="3">
+        <v>614</v>
+      </c>
+      <c r="B20" s="2">
+        <v>150817</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1112</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="3">
+        <v>613</v>
+      </c>
+      <c r="G20" s="7">
+        <v>150811</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1233</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
       <c r="M20" s="5"/>
@@ -1532,6 +1638,30 @@
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>614</v>
+      </c>
+      <c r="B21" s="2">
+        <v>150817</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1147</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3">
+        <v>613</v>
+      </c>
+      <c r="G21" s="7">
+        <v>150811</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1307</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
       <c r="M21" s="5"/>
@@ -1543,6 +1673,30 @@
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>614</v>
+      </c>
+      <c r="B22" s="2">
+        <v>150818</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1141</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>613</v>
+      </c>
+      <c r="G22" s="7">
+        <v>150812</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1307</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
       <c r="M22" s="5"/>
@@ -1554,6 +1708,30 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>614</v>
+      </c>
+      <c r="B23" s="2">
+        <v>150818</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1216</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3">
+        <v>613</v>
+      </c>
+      <c r="G23" s="7">
+        <v>150812</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1343</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="2"/>
       <c r="M23" s="5"/>
@@ -1565,6 +1743,30 @@
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>614</v>
+      </c>
+      <c r="B24" s="2">
+        <v>150819</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1032</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3">
+        <v>613</v>
+      </c>
+      <c r="G24" s="7">
+        <v>150813</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1646</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K24" s="3"/>
       <c r="L24" s="2"/>
       <c r="M24" s="5"/>
@@ -1576,6 +1778,30 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>614</v>
+      </c>
+      <c r="B25" s="2">
+        <v>150819</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>613</v>
+      </c>
+      <c r="G25" s="7">
+        <v>150817</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1253</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K25" s="3"/>
       <c r="L25" s="2"/>
       <c r="M25" s="5"/>
@@ -1587,6 +1813,30 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>614</v>
+      </c>
+      <c r="B26" s="2">
+        <v>150820</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1121</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>613</v>
+      </c>
+      <c r="G26" s="7">
+        <v>150817</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1333</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="2"/>
       <c r="M26" s="5"/>
@@ -1598,6 +1848,30 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>614</v>
+      </c>
+      <c r="B27" s="2">
+        <v>150820</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1157</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3">
+        <v>613</v>
+      </c>
+      <c r="G27" s="7">
+        <v>150818</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1259</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K27" s="3"/>
       <c r="L27" s="2"/>
       <c r="M27" s="5"/>
@@ -1609,6 +1883,30 @@
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>614</v>
+      </c>
+      <c r="B28" s="2">
+        <v>150821</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1107</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3">
+        <v>613</v>
+      </c>
+      <c r="G28" s="7">
+        <v>150818</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1335</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K28" s="3"/>
       <c r="L28" s="2"/>
       <c r="M28" s="5"/>
@@ -1620,6 +1918,30 @@
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>614</v>
+      </c>
+      <c r="B29" s="2">
+        <v>150821</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1143</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3">
+        <v>613</v>
+      </c>
+      <c r="G29" s="7">
+        <v>150819</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1151</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K29" s="3"/>
       <c r="L29" s="2"/>
       <c r="M29" s="5"/>
@@ -1631,6 +1953,30 @@
       <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>614</v>
+      </c>
+      <c r="B30" s="2">
+        <v>150823</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1355</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="3">
+        <v>613</v>
+      </c>
+      <c r="G30" s="7">
+        <v>150820</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1612</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="L30" s="2"/>
       <c r="M30" s="5"/>
@@ -1642,6 +1988,30 @@
       <c r="U30" s="5"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>614</v>
+      </c>
+      <c r="B31" s="2">
+        <v>150823</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1430</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="3">
+        <v>613</v>
+      </c>
+      <c r="G31" s="7">
+        <v>150820</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1653</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="2"/>
       <c r="M31" s="5"/>
@@ -1653,6 +2023,30 @@
       <c r="U31" s="5"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>614</v>
+      </c>
+      <c r="B32" s="4">
+        <v>150824</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1215</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="3">
+        <v>613</v>
+      </c>
+      <c r="G32" s="7">
+        <v>150821</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1224</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K32" s="3"/>
       <c r="L32" s="2"/>
       <c r="M32" s="5"/>
@@ -1663,7 +2057,31 @@
       <c r="T32" s="2"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>614</v>
+      </c>
+      <c r="B33" s="2">
+        <v>150827</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1035</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3">
+        <v>613</v>
+      </c>
+      <c r="G33" s="7">
+        <v>150821</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1301</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="2"/>
       <c r="M33" s="5"/>
@@ -1674,7 +2092,19 @@
       <c r="T33" s="2"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>614</v>
+      </c>
+      <c r="B34" s="2">
+        <v>150829</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1420</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="2"/>
       <c r="M34" s="5"/>
@@ -1685,7 +2115,19 @@
       <c r="T34" s="2"/>
       <c r="U34" s="5"/>
     </row>
-    <row r="35" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>614</v>
+      </c>
+      <c r="B35" s="2">
+        <v>150901</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1008</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="K35" s="3"/>
       <c r="L35" s="2"/>
       <c r="M35" s="5"/>
@@ -1696,7 +2138,20 @@
       <c r="T35" s="2"/>
       <c r="U35" s="5"/>
     </row>
-    <row r="36" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>614</v>
+      </c>
+      <c r="B36" s="2">
+        <v>150903</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1019</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1"/>
       <c r="K36" s="3"/>
       <c r="L36" s="2"/>
       <c r="M36" s="5"/>
@@ -1707,7 +2162,20 @@
       <c r="T36" s="2"/>
       <c r="U36" s="5"/>
     </row>
-    <row r="37" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>614</v>
+      </c>
+      <c r="B37" s="2">
+        <v>150905</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1416</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="1"/>
       <c r="K37" s="3"/>
       <c r="L37" s="2"/>
       <c r="M37" s="5"/>
@@ -1718,7 +2186,19 @@
       <c r="T37" s="2"/>
       <c r="U37" s="5"/>
     </row>
-    <row r="38" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>614</v>
+      </c>
+      <c r="B38" s="2">
+        <v>150908</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="K38" s="3"/>
       <c r="L38" s="2"/>
       <c r="M38" s="5"/>
@@ -1729,29 +2209,33 @@
       <c r="T38" s="2"/>
       <c r="U38" s="5"/>
     </row>
-    <row r="39" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K39" s="3"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="5"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="6"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="5"/>
-    </row>
-    <row r="40" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K40" s="3"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="5"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="6"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="5"/>
-    </row>
-    <row r="41" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="D39"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="5"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="6"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="5"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="D40"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="5"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="6"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="5"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K41" s="3"/>
       <c r="L41" s="2"/>
       <c r="M41" s="5"/>
@@ -1762,7 +2246,7 @@
       <c r="T41" s="2"/>
       <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K42" s="3"/>
       <c r="L42" s="2"/>
       <c r="M42" s="5"/>
@@ -1773,7 +2257,7 @@
       <c r="T42" s="2"/>
       <c r="U42" s="5"/>
     </row>
-    <row r="43" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K43" s="3"/>
       <c r="L43" s="2"/>
       <c r="M43" s="5"/>
@@ -1784,7 +2268,7 @@
       <c r="T43" s="2"/>
       <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K44" s="3"/>
       <c r="L44" s="2"/>
       <c r="M44" s="5"/>
@@ -1795,7 +2279,7 @@
       <c r="T44" s="2"/>
       <c r="U44" s="5"/>
     </row>
-    <row r="45" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K45" s="3"/>
       <c r="L45" s="2"/>
       <c r="M45" s="5"/>
@@ -1806,7 +2290,7 @@
       <c r="T45" s="2"/>
       <c r="U45" s="5"/>
     </row>
-    <row r="46" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K46" s="3"/>
       <c r="L46" s="2"/>
       <c r="M46" s="5"/>
@@ -1817,7 +2301,7 @@
       <c r="T46" s="2"/>
       <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K47" s="3"/>
       <c r="L47" s="2"/>
       <c r="M47" s="5"/>
@@ -1828,7 +2312,7 @@
       <c r="T47" s="2"/>
       <c r="U47" s="5"/>
     </row>
-    <row r="48" spans="11:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K48" s="3"/>
       <c r="L48" s="2"/>
       <c r="M48" s="5"/>
@@ -2161,8 +2645,9 @@
       <c r="M81" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D13">
-    <sortCondition ref="B2:B13"/>
+  <sortState ref="A2:D38">
+    <sortCondition ref="B2:B38"/>
+    <sortCondition ref="C2:C38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2174,7 +2659,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>